<commit_message>
coding 84  fixing key by excel
</commit_message>
<xml_diff>
--- a/Comercio.xlsx
+++ b/Comercio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandon/MyProjects/compareExcelEbcRuby/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7594924-A1EA-0546-8372-DE853028CCD6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC79F82-F87F-114E-8C0B-A9BF0697D451}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
   <si>
     <t>CLAVE</t>
   </si>
@@ -414,96 +414,6 @@
   </si>
   <si>
     <t>8° semestre</t>
-  </si>
-  <si>
-    <t>ICI27402</t>
-  </si>
-  <si>
-    <t>ICI27403</t>
-  </si>
-  <si>
-    <t>ICI27404</t>
-  </si>
-  <si>
-    <t>ICI27405</t>
-  </si>
-  <si>
-    <t>ICI27406</t>
-  </si>
-  <si>
-    <t>IPL27402</t>
-  </si>
-  <si>
-    <t>IPL27403</t>
-  </si>
-  <si>
-    <t>IPL27404</t>
-  </si>
-  <si>
-    <t>IPL27405</t>
-  </si>
-  <si>
-    <t>IPL27406</t>
-  </si>
-  <si>
-    <t>INI27402</t>
-  </si>
-  <si>
-    <t>INI27403</t>
-  </si>
-  <si>
-    <t>INI27404</t>
-  </si>
-  <si>
-    <t>INI27405</t>
-  </si>
-  <si>
-    <t>INI27406</t>
-  </si>
-  <si>
-    <t>ICI27604</t>
-  </si>
-  <si>
-    <t>ICI27605</t>
-  </si>
-  <si>
-    <t>ICI27606</t>
-  </si>
-  <si>
-    <t>ICI27607</t>
-  </si>
-  <si>
-    <t>ICI27608</t>
-  </si>
-  <si>
-    <t>IGA27604</t>
-  </si>
-  <si>
-    <t>IGA27605</t>
-  </si>
-  <si>
-    <t>IGA27606</t>
-  </si>
-  <si>
-    <t>IGA27607</t>
-  </si>
-  <si>
-    <t>IGA27608</t>
-  </si>
-  <si>
-    <t>IPL27604</t>
-  </si>
-  <si>
-    <t>IPL27605</t>
-  </si>
-  <si>
-    <t>IPL27606</t>
-  </si>
-  <si>
-    <t>IPL27607</t>
-  </si>
-  <si>
-    <t>IPL27608</t>
   </si>
   <si>
     <t xml:space="preserve">2.1  Leyes relacionadas con la legislación aduanera.
@@ -970,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1020,7 +930,7 @@
     </row>
     <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -1034,7 +944,7 @@
     </row>
     <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -1048,7 +958,7 @@
     </row>
     <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -1062,7 +972,7 @@
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -1076,7 +986,7 @@
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -1104,7 +1014,7 @@
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>20</v>
@@ -1118,7 +1028,7 @@
     </row>
     <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>20</v>
@@ -1132,7 +1042,7 @@
     </row>
     <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>20</v>
@@ -1146,7 +1056,7 @@
     </row>
     <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>20</v>
@@ -1160,7 +1070,7 @@
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>20</v>
@@ -1188,7 +1098,7 @@
     </row>
     <row r="16" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>34</v>
@@ -1202,7 +1112,7 @@
     </row>
     <row r="17" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>34</v>
@@ -1216,7 +1126,7 @@
     </row>
     <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>34</v>
@@ -1230,7 +1140,7 @@
     </row>
     <row r="19" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>34</v>
@@ -1244,7 +1154,7 @@
     </row>
     <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>34</v>
@@ -1378,7 +1288,7 @@
     </row>
     <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>50</v>
@@ -1392,7 +1302,7 @@
     </row>
     <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>50</v>
@@ -1406,7 +1316,7 @@
     </row>
     <row r="41" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>50</v>
@@ -1420,7 +1330,7 @@
     </row>
     <row r="42" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>50</v>
@@ -1434,7 +1344,7 @@
     </row>
     <row r="43" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>50</v>
@@ -1462,7 +1372,7 @@
     </row>
     <row r="45" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>64</v>
@@ -1471,12 +1381,12 @@
         <v>67</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>64</v>
@@ -1490,7 +1400,7 @@
     </row>
     <row r="47" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>64</v>
@@ -1504,7 +1414,7 @@
     </row>
     <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>64</v>
@@ -1518,7 +1428,7 @@
     </row>
     <row r="49" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>64</v>
@@ -1546,7 +1456,7 @@
     </row>
     <row r="51" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>77</v>
@@ -1560,7 +1470,7 @@
     </row>
     <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>77</v>
@@ -1574,7 +1484,7 @@
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>77</v>
@@ -1588,7 +1498,7 @@
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>77</v>
@@ -1602,7 +1512,7 @@
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>77</v>

</xml_diff>